<commit_message>
Update January 20 2021
</commit_message>
<xml_diff>
--- a/NombreDeCas.xlsx
+++ b/NombreDeCas.xlsx
@@ -223,7 +223,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -342,9 +342,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$11:$A$243</c:f>
+              <c:f>Feuil1!$A$11:$A$298</c:f>
               <c:strCache>
-                <c:ptCount val="233"/>
+                <c:ptCount val="288"/>
                 <c:pt idx="0">
                   <c:v>23-mars</c:v>
                 </c:pt>
@@ -1043,16 +1043,181 @@
                 </c:pt>
                 <c:pt idx="232">
                   <c:v>10-nov.</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>11-nov.</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>12-nov.</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>13-nov.</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>14-nov.</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>15-nov.</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>16-nov.</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>17-nov.</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>18-nov.</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>19-nov.</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>20-nov.</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>21-nov.</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>22-nov.</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>23-nov.</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>24-nov.</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>25-nov.</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>26-nov.</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>27-nov.</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>28-nov.</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>29-nov.</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>30-nov.</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>01-déc.</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>02-déc.</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>03-déc.</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>04-déc.</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>05-déc.</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>06-déc.</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>07-déc.</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>08-déc.</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>09-déc.</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>10-déc.</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>11-déc.</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>12-déc.</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>13-déc.</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>14-déc.</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>15-déc.</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>16-déc.</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>17-déc.</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>18-déc.</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>19-déc.</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>20-déc.</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>21-déc.</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>22-déc.</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>23-déc.</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>24-déc.</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>25-déc.</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>26-déc.</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>27-déc.</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>28-déc.</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>29-déc.</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>30-déc.</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>31-déc.</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>01-janv.</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>02-janv.</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>03-janv.</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>04-janv.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$D$11:$D$243</c:f>
+              <c:f>Feuil1!$D$11:$D$298</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="233"/>
+                <c:ptCount val="288"/>
                 <c:pt idx="0">
                   <c:v>628</c:v>
                 </c:pt>
@@ -1751,6 +1916,171 @@
                 </c:pt>
                 <c:pt idx="232">
                   <c:v>117151</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>118529</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>119894</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>121195</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>122643</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>123854</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>125072</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>126054</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>127233</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>128440</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>129699</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>130888</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>132042</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>133206</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>134330</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>135430</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>136894</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>138163</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>139643</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>141038</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>142371</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>143548</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>145062</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>146532</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>147877</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>149908</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>151599</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>153176</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>154740</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>156468</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>158310</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>160023</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>161921</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>163915</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>165535</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>167276</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>169173</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>171028</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>172801</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>174839</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>176985</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>179093</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>181276</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>183523</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>185872</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>188118</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>190364</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>192655</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>194930</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>197311</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>199822</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>202641</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>205449</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>207435</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>210304</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>212850</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1758,11 +2088,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="61700767"/>
-        <c:axId val="11778487"/>
+        <c:axId val="5257190"/>
+        <c:axId val="79032723"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61700767"/>
+        <c:axId val="5257190"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1794,7 +2124,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11778487"/>
+        <c:crossAx val="79032723"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1802,7 +2132,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11778487"/>
+        <c:axId val="79032723"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1841,7 +2171,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61700767"/>
+        <c:crossAx val="5257190"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1869,7 +2199,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1952,9 +2282,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$3:$A$243</c:f>
+              <c:f>Feuil1!$A$3:$A$298</c:f>
               <c:strCache>
-                <c:ptCount val="241"/>
+                <c:ptCount val="296"/>
                 <c:pt idx="0">
                   <c:v>15-mars</c:v>
                 </c:pt>
@@ -2677,16 +3007,181 @@
                 </c:pt>
                 <c:pt idx="240">
                   <c:v>10-nov.</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>11-nov.</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>12-nov.</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>13-nov.</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>14-nov.</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>15-nov.</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>16-nov.</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>17-nov.</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>18-nov.</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>19-nov.</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>20-nov.</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>21-nov.</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>22-nov.</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>23-nov.</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>24-nov.</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>25-nov.</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>26-nov.</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>27-nov.</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>28-nov.</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>29-nov.</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>30-nov.</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>01-déc.</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>02-déc.</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>03-déc.</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>04-déc.</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>05-déc.</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>06-déc.</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>07-déc.</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>08-déc.</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>09-déc.</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>10-déc.</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>11-déc.</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>12-déc.</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>13-déc.</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>14-déc.</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>15-déc.</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>16-déc.</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>17-déc.</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>18-déc.</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>19-déc.</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>20-déc.</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>21-déc.</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>22-déc.</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>23-déc.</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>24-déc.</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>25-déc.</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>26-déc.</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>27-déc.</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>28-déc.</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>29-déc.</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>30-déc.</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>31-déc.</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>01-janv.</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>02-janv.</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>03-janv.</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>04-janv.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$E$3:$E$243</c:f>
+              <c:f>Feuil1!$E$3:$E$298</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="241"/>
+                <c:ptCount val="296"/>
                 <c:pt idx="0">
                   <c:v>15</c:v>
                 </c:pt>
@@ -3409,6 +3904,171 @@
                 </c:pt>
                 <c:pt idx="240">
                   <c:v>1162</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>1378</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>1365</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>1301</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>1448</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>1211</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>1218</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>982</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>1179</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>1207</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1259</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>1189</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>1154</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>1164</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>1124</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>1464</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>1269</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>1480</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>1395</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>1333</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>1177</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>1514</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>1470</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>1345</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>1691</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>1577</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>1564</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>1728</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>1842</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>1713</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>1898</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>1620</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>1741</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>1897</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>1773</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>2146</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>2108</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>2183</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>2247</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>2349</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>2246</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>2246</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>2291</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>2275</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>2381</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>2511</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>2819</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>2808</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>2869</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>2546</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3416,11 +4076,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="39698773"/>
-        <c:axId val="49683796"/>
+        <c:axId val="86187282"/>
+        <c:axId val="49761413"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39698773"/>
+        <c:axId val="86187282"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3452,7 +4112,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49683796"/>
+        <c:crossAx val="49761413"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3460,7 +4120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49683796"/>
+        <c:axId val="49761413"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3499,7 +4159,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39698773"/>
+        <c:crossAx val="86187282"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3527,7 +4187,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3611,9 +4271,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$5:$A$243</c:f>
+              <c:f>Feuil1!$A$5:$A$298</c:f>
               <c:strCache>
-                <c:ptCount val="239"/>
+                <c:ptCount val="294"/>
                 <c:pt idx="0">
                   <c:v>17-mars</c:v>
                 </c:pt>
@@ -4330,16 +4990,181 @@
                 </c:pt>
                 <c:pt idx="238">
                   <c:v>10-nov.</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>11-nov.</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>12-nov.</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>13-nov.</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>14-nov.</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>15-nov.</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>16-nov.</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>17-nov.</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>18-nov.</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>19-nov.</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>20-nov.</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>21-nov.</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>22-nov.</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>23-nov.</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>24-nov.</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>25-nov.</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>26-nov.</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>27-nov.</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>28-nov.</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>29-nov.</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>30-nov.</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>01-déc.</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>02-déc.</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>03-déc.</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>04-déc.</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>05-déc.</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>06-déc.</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>07-déc.</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>08-déc.</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>09-déc.</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>10-déc.</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>11-déc.</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>12-déc.</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>13-déc.</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>14-déc.</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>15-déc.</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>16-déc.</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>17-déc.</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>18-déc.</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>19-déc.</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>20-déc.</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>21-déc.</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>22-déc.</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>23-déc.</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>24-déc.</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>25-déc.</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>26-déc.</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>27-déc.</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>28-déc.</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>29-déc.</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>30-déc.</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>31-déc.</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>01-janv.</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>02-janv.</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>03-janv.</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>04-janv.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$F$5:$F$243</c:f>
+              <c:f>Feuil1!$F$5:$F$298</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="239"/>
+                <c:ptCount val="294"/>
                 <c:pt idx="0">
                   <c:v>16.6666666666667</c:v>
                 </c:pt>
@@ -5056,6 +5881,171 @@
                 </c:pt>
                 <c:pt idx="238">
                   <c:v>1242.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>1236.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>1301.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>1348</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>1371.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>1292.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>1137</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>1126.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>1122.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>1215</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>1218.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1200.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>1169</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>1147.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>1129.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>1229.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>1277.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>1404.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>1381.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>1402.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>1301.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>1341.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>1387</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>1443</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>1615.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>1689</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>1766.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>1610.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>1623</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>1711.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>1761</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>1817.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>1868.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>1837.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>1785</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>1752.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>1831</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>1841.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>1888.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>1985.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>2097.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>2145.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>2179.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>2259.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>2280.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>2280.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>2261</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>2270.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>2315.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>2389</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>2570.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>2712.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>2537.66666666667</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>2554.33333333333</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>2467</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5063,11 +6053,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="21666693"/>
-        <c:axId val="98560636"/>
+        <c:axId val="78820550"/>
+        <c:axId val="8332950"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="21666693"/>
+        <c:axId val="78820550"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5099,7 +6089,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98560636"/>
+        <c:crossAx val="8332950"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5107,7 +6097,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98560636"/>
+        <c:axId val="8332950"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5146,7 +6136,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21666693"/>
+        <c:crossAx val="78820550"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5174,7 +6164,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5295,9 +6285,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$9:$A$243</c:f>
+              <c:f>Feuil1!$A$9:$A$298</c:f>
               <c:strCache>
-                <c:ptCount val="235"/>
+                <c:ptCount val="290"/>
                 <c:pt idx="0">
                   <c:v>21-mars</c:v>
                 </c:pt>
@@ -6002,16 +6992,181 @@
                 </c:pt>
                 <c:pt idx="234">
                   <c:v>10-nov.</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>11-nov.</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>12-nov.</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>13-nov.</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>14-nov.</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>15-nov.</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>16-nov.</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>17-nov.</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>18-nov.</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>19-nov.</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>20-nov.</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>21-nov.</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>22-nov.</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>23-nov.</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>24-nov.</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>25-nov.</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>26-nov.</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>27-nov.</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>28-nov.</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>29-nov.</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>30-nov.</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>01-déc.</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>02-déc.</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>03-déc.</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>04-déc.</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>05-déc.</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>06-déc.</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>07-déc.</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>08-déc.</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>09-déc.</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>10-déc.</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>11-déc.</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>12-déc.</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>13-déc.</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>14-déc.</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>15-déc.</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>16-déc.</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>17-déc.</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>18-déc.</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>19-déc.</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>20-déc.</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>21-déc.</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>22-déc.</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>23-déc.</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>24-déc.</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>25-déc.</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>26-déc.</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>27-déc.</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>28-déc.</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>29-déc.</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>30-déc.</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>31-déc.</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>01-janv.</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>02-janv.</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>03-janv.</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>04-janv.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$G$9:$G$243</c:f>
+              <c:f>Feuil1!$G$9:$G$298</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="235"/>
+                <c:ptCount val="290"/>
                 <c:pt idx="0">
                   <c:v>22.4285714285714</c:v>
                 </c:pt>
@@ -6716,6 +7871,171 @@
                 </c:pt>
                 <c:pt idx="234">
                   <c:v>1180.28571428571</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>1230.14285714286</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>1262.57142857143</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>1286.57142857143</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>1317.14285714286</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>1290.57142857143</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>1297.57142857143</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>1271.85714285714</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>1243.42857142857</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>1220.85714285714</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>1214.85714285714</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>1177.85714285714</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>1169.71428571429</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>1162</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>1182.28571428571</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>1171</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1207.71428571429</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>1209.14285714286</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>1250.71428571429</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>1285.14285714286</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>1309.28571428571</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>1316.85714285714</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>1376</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>1376.85714285714</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>1387.71428571429</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>1466.42857142857</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>1508.71428571429</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>1543.57142857143</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>1598.85714285714</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>1629.42857142857</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>1682.57142857143</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>1735.14285714286</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>1716.14285714286</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>1759.42857142857</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>1765.57142857143</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>1790.85714285714</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>1815</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>1816.85714285714</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>1825.42857142857</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>1845.42857142857</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>1867.14285714286</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>1936.85714285714</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>2120.57142857143</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>2188.14285714286</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>2217.85714285714</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>2238.57142857143</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>2262.42857142857</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>2290.71428571429</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>2328.42857142857</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>2395.57142857143</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>2475.85714285714</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>2438.71428571429</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>2521.28571428571</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>2560</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6723,11 +8043,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="81107285"/>
-        <c:axId val="8969373"/>
+        <c:axId val="27955286"/>
+        <c:axId val="58841941"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81107285"/>
+        <c:axId val="27955286"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6759,7 +8079,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8969373"/>
+        <c:crossAx val="58841941"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6767,7 +8087,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8969373"/>
+        <c:axId val="58841941"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6806,7 +8126,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81107285"/>
+        <c:crossAx val="27955286"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6841,13 +8161,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>428760</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>419400</xdr:colOff>
+      <xdr:colOff>402840</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
+      <xdr:rowOff>54000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6855,8 +8175,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7926840" y="1716840"/>
-        <a:ext cx="5614200" cy="2733840"/>
+        <a:off x="7926840" y="1717920"/>
+        <a:ext cx="5597640" cy="2717280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6871,13 +8191,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>647640</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>11880</xdr:rowOff>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>638280</xdr:colOff>
+      <xdr:colOff>621720</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:rowOff>63360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6885,8 +8205,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13769280" y="1726200"/>
-        <a:ext cx="5614200" cy="2733840"/>
+        <a:off x="13769280" y="1727280"/>
+        <a:ext cx="5597640" cy="2717280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6899,15 +8219,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>2520</xdr:colOff>
+      <xdr:colOff>3600</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>744120</xdr:colOff>
+      <xdr:colOff>728640</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>97920</xdr:rowOff>
+      <xdr:rowOff>82440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6915,8 +8235,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8437680" y="5145840"/>
-        <a:ext cx="10114200" cy="3143520"/>
+        <a:off x="8438760" y="5146920"/>
+        <a:ext cx="10097640" cy="3126960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6929,15 +8249,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>2520</xdr:colOff>
+      <xdr:colOff>3600</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>732600</xdr:colOff>
+      <xdr:colOff>717120</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>97920</xdr:rowOff>
+      <xdr:rowOff>82440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6945,8 +8265,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8437680" y="8574840"/>
-        <a:ext cx="10102680" cy="3143520"/>
+        <a:off x="8438760" y="8575920"/>
+        <a:ext cx="10086120" cy="3126960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6964,10 +8284,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J300"/>
+  <dimension ref="A1:J330"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C34" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R72" activeCellId="0" sqref="R72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A301" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B315" activeCellId="0" sqref="B315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13546,21 +14866,24 @@
         <f aca="false">$A243+1</f>
         <v>44146</v>
       </c>
+      <c r="B244" s="0" t="n">
+        <v>118529</v>
+      </c>
       <c r="D244" s="1" t="n">
         <f aca="false">B244+C244</f>
-        <v>0</v>
+        <v>118529</v>
       </c>
       <c r="E244" s="1" t="n">
         <f aca="false">D244-D243</f>
-        <v>-117151</v>
+        <v>1378</v>
       </c>
       <c r="F244" s="1" t="n">
         <f aca="false">(E242+E243+E244)/3</f>
-        <v>-38273.3333333333</v>
+        <v>1236.33333333333</v>
       </c>
       <c r="G244" s="1" t="n">
         <f aca="false">(E238+E239+E240+E241+E242+E243+E244)/7</f>
-        <v>-15702.5714285714</v>
+        <v>1230.14285714286</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13568,21 +14891,24 @@
         <f aca="false">$A244+1</f>
         <v>44147</v>
       </c>
+      <c r="B245" s="0" t="n">
+        <v>119894</v>
+      </c>
       <c r="D245" s="1" t="n">
         <f aca="false">B245+C245</f>
-        <v>0</v>
+        <v>119894</v>
       </c>
       <c r="E245" s="1" t="n">
         <f aca="false">D245-D244</f>
-        <v>0</v>
+        <v>1365</v>
       </c>
       <c r="F245" s="1" t="n">
         <f aca="false">(E243+E244+E245)/3</f>
-        <v>-38663</v>
+        <v>1301.66666666667</v>
       </c>
       <c r="G245" s="1" t="n">
         <f aca="false">(E239+E240+E241+E242+E243+E244+E245)/7</f>
-        <v>-15865.1428571429</v>
+        <v>1262.57142857143</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13590,21 +14916,24 @@
         <f aca="false">$A245+1</f>
         <v>44148</v>
       </c>
+      <c r="B246" s="0" t="n">
+        <v>121195</v>
+      </c>
       <c r="D246" s="1" t="n">
         <f aca="false">B246+C246</f>
-        <v>0</v>
+        <v>121195</v>
       </c>
       <c r="E246" s="1" t="n">
         <f aca="false">D246-D245</f>
-        <v>0</v>
+        <v>1301</v>
       </c>
       <c r="F246" s="1" t="n">
         <f aca="false">(E244+E245+E246)/3</f>
-        <v>-39050.3333333333</v>
+        <v>1348</v>
       </c>
       <c r="G246" s="1" t="n">
         <f aca="false">(E240+E241+E242+E243+E244+E245+E246)/7</f>
-        <v>-16027</v>
+        <v>1286.57142857143</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13612,21 +14941,24 @@
         <f aca="false">$A246+1</f>
         <v>44149</v>
       </c>
+      <c r="B247" s="0" t="n">
+        <v>122643</v>
+      </c>
       <c r="D247" s="1" t="n">
         <f aca="false">B247+C247</f>
-        <v>0</v>
+        <v>122643</v>
       </c>
       <c r="E247" s="1" t="n">
         <f aca="false">D247-D246</f>
-        <v>0</v>
+        <v>1448</v>
       </c>
       <c r="F247" s="1" t="n">
         <f aca="false">(E245+E246+E247)/3</f>
-        <v>0</v>
+        <v>1371.33333333333</v>
       </c>
       <c r="G247" s="1" t="n">
         <f aca="false">(E241+E242+E243+E244+E245+E246+E247)/7</f>
-        <v>-16203.2857142857</v>
+        <v>1317.14285714286</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13634,43 +14966,49 @@
         <f aca="false">$A247+1</f>
         <v>44150</v>
       </c>
+      <c r="B248" s="0" t="n">
+        <v>123854</v>
+      </c>
       <c r="D248" s="1" t="n">
         <f aca="false">B248+C248</f>
-        <v>0</v>
+        <v>123854</v>
       </c>
       <c r="E248" s="1" t="n">
         <f aca="false">D248-D247</f>
-        <v>0</v>
+        <v>1211</v>
       </c>
       <c r="F248" s="1" t="n">
         <f aca="false">(E246+E247+E248)/3</f>
-        <v>0</v>
+        <v>1320</v>
       </c>
       <c r="G248" s="1" t="n">
         <f aca="false">(E242+E243+E244+E245+E246+E247+E248)/7</f>
-        <v>-16402.8571428571</v>
-      </c>
-    </row>
-    <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1290.57142857143</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="n">
         <f aca="false">$A248+1</f>
         <v>44151</v>
       </c>
+      <c r="B249" s="0" t="n">
+        <v>125072</v>
+      </c>
       <c r="D249" s="1" t="n">
         <f aca="false">B249+C249</f>
-        <v>0</v>
+        <v>125072</v>
       </c>
       <c r="E249" s="1" t="n">
         <f aca="false">D249-D248</f>
-        <v>0</v>
+        <v>1218</v>
       </c>
       <c r="F249" s="1" t="n">
         <f aca="false">(E247+E248+E249)/3</f>
-        <v>0</v>
+        <v>1292.33333333333</v>
       </c>
       <c r="G249" s="1" t="n">
         <f aca="false">(E243+E244+E245+E246+E247+E248+E249)/7</f>
-        <v>-16569.8571428571</v>
+        <v>1297.57142857143</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13678,21 +15016,24 @@
         <f aca="false">$A249+1</f>
         <v>44152</v>
       </c>
+      <c r="B250" s="0" t="n">
+        <v>126054</v>
+      </c>
       <c r="D250" s="1" t="n">
         <f aca="false">B250+C250</f>
-        <v>0</v>
+        <v>126054</v>
       </c>
       <c r="E250" s="1" t="n">
         <f aca="false">D250-D249</f>
-        <v>0</v>
+        <v>982</v>
       </c>
       <c r="F250" s="1" t="n">
         <f aca="false">(E248+E249+E250)/3</f>
-        <v>0</v>
+        <v>1137</v>
       </c>
       <c r="G250" s="1" t="n">
         <f aca="false">(E244+E245+E246+E247+E248+E249+E250)/7</f>
-        <v>-16735.8571428571</v>
+        <v>1271.85714285714</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13700,21 +15041,24 @@
         <f aca="false">$A250+1</f>
         <v>44153</v>
       </c>
+      <c r="B251" s="0" t="n">
+        <v>127233</v>
+      </c>
       <c r="D251" s="1" t="n">
         <f aca="false">B251+C251</f>
-        <v>0</v>
+        <v>127233</v>
       </c>
       <c r="E251" s="1" t="n">
         <f aca="false">D251-D250</f>
-        <v>0</v>
+        <v>1179</v>
       </c>
       <c r="F251" s="1" t="n">
         <f aca="false">(E249+E250+E251)/3</f>
-        <v>0</v>
+        <v>1126.33333333333</v>
       </c>
       <c r="G251" s="1" t="n">
         <f aca="false">(E245+E246+E247+E248+E249+E250+E251)/7</f>
-        <v>0</v>
+        <v>1243.42857142857</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13722,21 +15066,24 @@
         <f aca="false">$A251+1</f>
         <v>44154</v>
       </c>
+      <c r="B252" s="0" t="n">
+        <v>128440</v>
+      </c>
       <c r="D252" s="1" t="n">
         <f aca="false">B252+C252</f>
-        <v>0</v>
+        <v>128440</v>
       </c>
       <c r="E252" s="1" t="n">
         <f aca="false">D252-D251</f>
-        <v>0</v>
+        <v>1207</v>
       </c>
       <c r="F252" s="1" t="n">
         <f aca="false">(E250+E251+E252)/3</f>
-        <v>0</v>
+        <v>1122.66666666667</v>
       </c>
       <c r="G252" s="1" t="n">
         <f aca="false">(E246+E247+E248+E249+E250+E251+E252)/7</f>
-        <v>0</v>
+        <v>1220.85714285714</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13744,21 +15091,24 @@
         <f aca="false">$A252+1</f>
         <v>44155</v>
       </c>
+      <c r="B253" s="0" t="n">
+        <v>129699</v>
+      </c>
       <c r="D253" s="1" t="n">
         <f aca="false">B253+C253</f>
-        <v>0</v>
+        <v>129699</v>
       </c>
       <c r="E253" s="1" t="n">
         <f aca="false">D253-D252</f>
-        <v>0</v>
+        <v>1259</v>
       </c>
       <c r="F253" s="1" t="n">
         <f aca="false">(E251+E252+E253)/3</f>
-        <v>0</v>
+        <v>1215</v>
       </c>
       <c r="G253" s="1" t="n">
         <f aca="false">(E247+E248+E249+E250+E251+E252+E253)/7</f>
-        <v>0</v>
+        <v>1214.85714285714</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13766,21 +15116,24 @@
         <f aca="false">$A253+1</f>
         <v>44156</v>
       </c>
+      <c r="B254" s="0" t="n">
+        <v>130888</v>
+      </c>
       <c r="D254" s="1" t="n">
         <f aca="false">B254+C254</f>
-        <v>0</v>
+        <v>130888</v>
       </c>
       <c r="E254" s="1" t="n">
         <f aca="false">D254-D253</f>
-        <v>0</v>
+        <v>1189</v>
       </c>
       <c r="F254" s="1" t="n">
         <f aca="false">(E252+E253+E254)/3</f>
-        <v>0</v>
+        <v>1218.33333333333</v>
       </c>
       <c r="G254" s="1" t="n">
         <f aca="false">(E248+E249+E250+E251+E252+E253+E254)/7</f>
-        <v>0</v>
+        <v>1177.85714285714</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13788,21 +15141,24 @@
         <f aca="false">$A254+1</f>
         <v>44157</v>
       </c>
+      <c r="B255" s="0" t="n">
+        <v>132042</v>
+      </c>
       <c r="D255" s="1" t="n">
         <f aca="false">B255+C255</f>
-        <v>0</v>
+        <v>132042</v>
       </c>
       <c r="E255" s="1" t="n">
         <f aca="false">D255-D254</f>
-        <v>0</v>
+        <v>1154</v>
       </c>
       <c r="F255" s="1" t="n">
         <f aca="false">(E253+E254+E255)/3</f>
-        <v>0</v>
+        <v>1200.66666666667</v>
       </c>
       <c r="G255" s="1" t="n">
         <f aca="false">(E249+E250+E251+E252+E253+E254+E255)/7</f>
-        <v>0</v>
+        <v>1169.71428571429</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13810,21 +15166,24 @@
         <f aca="false">$A255+1</f>
         <v>44158</v>
       </c>
+      <c r="B256" s="0" t="n">
+        <v>133206</v>
+      </c>
       <c r="D256" s="1" t="n">
         <f aca="false">B256+C256</f>
-        <v>0</v>
+        <v>133206</v>
       </c>
       <c r="E256" s="1" t="n">
         <f aca="false">D256-D255</f>
-        <v>0</v>
+        <v>1164</v>
       </c>
       <c r="F256" s="1" t="n">
         <f aca="false">(E254+E255+E256)/3</f>
-        <v>0</v>
+        <v>1169</v>
       </c>
       <c r="G256" s="1" t="n">
         <f aca="false">(E250+E251+E252+E253+E254+E255+E256)/7</f>
-        <v>0</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13832,21 +15191,24 @@
         <f aca="false">$A256+1</f>
         <v>44159</v>
       </c>
+      <c r="B257" s="0" t="n">
+        <v>134330</v>
+      </c>
       <c r="D257" s="1" t="n">
         <f aca="false">B257+C257</f>
-        <v>0</v>
+        <v>134330</v>
       </c>
       <c r="E257" s="1" t="n">
         <f aca="false">D257-D256</f>
-        <v>0</v>
+        <v>1124</v>
       </c>
       <c r="F257" s="1" t="n">
         <f aca="false">(E255+E256+E257)/3</f>
-        <v>0</v>
+        <v>1147.33333333333</v>
       </c>
       <c r="G257" s="1" t="n">
         <f aca="false">(E251+E252+E253+E254+E255+E256+E257)/7</f>
-        <v>0</v>
+        <v>1182.28571428571</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13854,21 +15216,24 @@
         <f aca="false">$A257+1</f>
         <v>44160</v>
       </c>
+      <c r="B258" s="0" t="n">
+        <v>135430</v>
+      </c>
       <c r="D258" s="1" t="n">
         <f aca="false">B258+C258</f>
-        <v>0</v>
+        <v>135430</v>
       </c>
       <c r="E258" s="1" t="n">
         <f aca="false">D258-D257</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="F258" s="1" t="n">
         <f aca="false">(E256+E257+E258)/3</f>
-        <v>0</v>
+        <v>1129.33333333333</v>
       </c>
       <c r="G258" s="1" t="n">
         <f aca="false">(E252+E253+E254+E255+E256+E257+E258)/7</f>
-        <v>0</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13876,21 +15241,24 @@
         <f aca="false">$A258+1</f>
         <v>44161</v>
       </c>
+      <c r="B259" s="0" t="n">
+        <v>136894</v>
+      </c>
       <c r="D259" s="1" t="n">
         <f aca="false">B259+C259</f>
-        <v>0</v>
+        <v>136894</v>
       </c>
       <c r="E259" s="1" t="n">
         <f aca="false">D259-D258</f>
-        <v>0</v>
+        <v>1464</v>
       </c>
       <c r="F259" s="1" t="n">
         <f aca="false">(E257+E258+E259)/3</f>
-        <v>0</v>
+        <v>1229.33333333333</v>
       </c>
       <c r="G259" s="1" t="n">
         <f aca="false">(E253+E254+E255+E256+E257+E258+E259)/7</f>
-        <v>0</v>
+        <v>1207.71428571429</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13898,21 +15266,24 @@
         <f aca="false">$A259+1</f>
         <v>44162</v>
       </c>
+      <c r="B260" s="0" t="n">
+        <v>138163</v>
+      </c>
       <c r="D260" s="1" t="n">
         <f aca="false">B260+C260</f>
-        <v>0</v>
+        <v>138163</v>
       </c>
       <c r="E260" s="1" t="n">
         <f aca="false">D260-D259</f>
-        <v>0</v>
+        <v>1269</v>
       </c>
       <c r="F260" s="1" t="n">
         <f aca="false">(E258+E259+E260)/3</f>
-        <v>0</v>
+        <v>1277.66666666667</v>
       </c>
       <c r="G260" s="1" t="n">
         <f aca="false">(E254+E255+E256+E257+E258+E259+E260)/7</f>
-        <v>0</v>
+        <v>1209.14285714286</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13920,21 +15291,24 @@
         <f aca="false">$A260+1</f>
         <v>44163</v>
       </c>
+      <c r="B261" s="0" t="n">
+        <v>139643</v>
+      </c>
       <c r="D261" s="1" t="n">
         <f aca="false">B261+C261</f>
-        <v>0</v>
+        <v>139643</v>
       </c>
       <c r="E261" s="1" t="n">
         <f aca="false">D261-D260</f>
-        <v>0</v>
+        <v>1480</v>
       </c>
       <c r="F261" s="1" t="n">
         <f aca="false">(E259+E260+E261)/3</f>
-        <v>0</v>
+        <v>1404.33333333333</v>
       </c>
       <c r="G261" s="1" t="n">
         <f aca="false">(E255+E256+E257+E258+E259+E260+E261)/7</f>
-        <v>0</v>
+        <v>1250.71428571429</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13942,43 +15316,49 @@
         <f aca="false">$A261+1</f>
         <v>44164</v>
       </c>
+      <c r="B262" s="0" t="n">
+        <v>141038</v>
+      </c>
       <c r="D262" s="1" t="n">
         <f aca="false">B262+C262</f>
-        <v>0</v>
+        <v>141038</v>
       </c>
       <c r="E262" s="1" t="n">
         <f aca="false">D262-D261</f>
-        <v>0</v>
+        <v>1395</v>
       </c>
       <c r="F262" s="1" t="n">
         <f aca="false">(E260+E261+E262)/3</f>
-        <v>0</v>
+        <v>1381.33333333333</v>
       </c>
       <c r="G262" s="1" t="n">
         <f aca="false">(E256+E257+E258+E259+E260+E261+E262)/7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1285.14285714286</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="2" t="n">
         <f aca="false">$A262+1</f>
         <v>44165</v>
       </c>
+      <c r="B263" s="0" t="n">
+        <v>142371</v>
+      </c>
       <c r="D263" s="1" t="n">
         <f aca="false">B263+C263</f>
-        <v>0</v>
+        <v>142371</v>
       </c>
       <c r="E263" s="1" t="n">
         <f aca="false">D263-D262</f>
-        <v>0</v>
+        <v>1333</v>
       </c>
       <c r="F263" s="1" t="n">
         <f aca="false">(E261+E262+E263)/3</f>
-        <v>0</v>
+        <v>1402.66666666667</v>
       </c>
       <c r="G263" s="1" t="n">
         <f aca="false">(E257+E258+E259+E260+E261+E262+E263)/7</f>
-        <v>0</v>
+        <v>1309.28571428571</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13986,21 +15366,24 @@
         <f aca="false">$A263+1</f>
         <v>44166</v>
       </c>
+      <c r="B264" s="0" t="n">
+        <v>143548</v>
+      </c>
       <c r="D264" s="1" t="n">
         <f aca="false">B264+C264</f>
-        <v>0</v>
+        <v>143548</v>
       </c>
       <c r="E264" s="1" t="n">
         <f aca="false">D264-D263</f>
-        <v>0</v>
+        <v>1177</v>
       </c>
       <c r="F264" s="1" t="n">
         <f aca="false">(E262+E263+E264)/3</f>
-        <v>0</v>
+        <v>1301.66666666667</v>
       </c>
       <c r="G264" s="1" t="n">
         <f aca="false">(E258+E259+E260+E261+E262+E263+E264)/7</f>
-        <v>0</v>
+        <v>1316.85714285714</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14008,21 +15391,24 @@
         <f aca="false">$A264+1</f>
         <v>44167</v>
       </c>
+      <c r="B265" s="0" t="n">
+        <v>145062</v>
+      </c>
       <c r="D265" s="1" t="n">
         <f aca="false">B265+C265</f>
-        <v>0</v>
+        <v>145062</v>
       </c>
       <c r="E265" s="1" t="n">
         <f aca="false">D265-D264</f>
-        <v>0</v>
+        <v>1514</v>
       </c>
       <c r="F265" s="1" t="n">
         <f aca="false">(E263+E264+E265)/3</f>
-        <v>0</v>
+        <v>1341.33333333333</v>
       </c>
       <c r="G265" s="1" t="n">
         <f aca="false">(E259+E260+E261+E262+E263+E264+E265)/7</f>
-        <v>0</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14030,21 +15416,24 @@
         <f aca="false">$A265+1</f>
         <v>44168</v>
       </c>
+      <c r="B266" s="0" t="n">
+        <v>146532</v>
+      </c>
       <c r="D266" s="1" t="n">
         <f aca="false">B266+C266</f>
-        <v>0</v>
+        <v>146532</v>
       </c>
       <c r="E266" s="1" t="n">
         <f aca="false">D266-D265</f>
-        <v>0</v>
+        <v>1470</v>
       </c>
       <c r="F266" s="1" t="n">
         <f aca="false">(E264+E265+E266)/3</f>
-        <v>0</v>
+        <v>1387</v>
       </c>
       <c r="G266" s="1" t="n">
         <f aca="false">(E260+E261+E262+E263+E264+E265+E266)/7</f>
-        <v>0</v>
+        <v>1376.85714285714</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14052,21 +15441,24 @@
         <f aca="false">$A266+1</f>
         <v>44169</v>
       </c>
+      <c r="B267" s="0" t="n">
+        <v>147877</v>
+      </c>
       <c r="D267" s="1" t="n">
         <f aca="false">B267+C267</f>
-        <v>0</v>
+        <v>147877</v>
       </c>
       <c r="E267" s="1" t="n">
         <f aca="false">D267-D266</f>
-        <v>0</v>
+        <v>1345</v>
       </c>
       <c r="F267" s="1" t="n">
         <f aca="false">(E265+E266+E267)/3</f>
-        <v>0</v>
+        <v>1443</v>
       </c>
       <c r="G267" s="1" t="n">
         <f aca="false">(E261+E262+E263+E264+E265+E266+E267)/7</f>
-        <v>0</v>
+        <v>1387.71428571429</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14074,21 +15466,24 @@
         <f aca="false">$A267+1</f>
         <v>44170</v>
       </c>
+      <c r="B268" s="0" t="n">
+        <v>149908</v>
+      </c>
       <c r="D268" s="1" t="n">
         <f aca="false">B268+C268</f>
-        <v>0</v>
+        <v>149908</v>
       </c>
       <c r="E268" s="1" t="n">
         <f aca="false">D268-D267</f>
-        <v>0</v>
+        <v>2031</v>
       </c>
       <c r="F268" s="1" t="n">
         <f aca="false">(E266+E267+E268)/3</f>
-        <v>0</v>
+        <v>1615.33333333333</v>
       </c>
       <c r="G268" s="1" t="n">
         <f aca="false">(E262+E263+E264+E265+E266+E267+E268)/7</f>
-        <v>0</v>
+        <v>1466.42857142857</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14096,21 +15491,24 @@
         <f aca="false">$A268+1</f>
         <v>44171</v>
       </c>
+      <c r="B269" s="0" t="n">
+        <v>151599</v>
+      </c>
       <c r="D269" s="1" t="n">
         <f aca="false">B269+C269</f>
-        <v>0</v>
+        <v>151599</v>
       </c>
       <c r="E269" s="1" t="n">
         <f aca="false">D269-D268</f>
-        <v>0</v>
+        <v>1691</v>
       </c>
       <c r="F269" s="1" t="n">
         <f aca="false">(E267+E268+E269)/3</f>
-        <v>0</v>
+        <v>1689</v>
       </c>
       <c r="G269" s="1" t="n">
         <f aca="false">(E263+E264+E265+E266+E267+E268+E269)/7</f>
-        <v>0</v>
+        <v>1508.71428571429</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14118,21 +15516,24 @@
         <f aca="false">$A269+1</f>
         <v>44172</v>
       </c>
+      <c r="B270" s="0" t="n">
+        <v>153176</v>
+      </c>
       <c r="D270" s="1" t="n">
         <f aca="false">B270+C270</f>
-        <v>0</v>
+        <v>153176</v>
       </c>
       <c r="E270" s="1" t="n">
         <f aca="false">D270-D269</f>
-        <v>0</v>
+        <v>1577</v>
       </c>
       <c r="F270" s="1" t="n">
         <f aca="false">(E268+E269+E270)/3</f>
-        <v>0</v>
+        <v>1766.33333333333</v>
       </c>
       <c r="G270" s="1" t="n">
         <f aca="false">(E264+E265+E266+E267+E268+E269+E270)/7</f>
-        <v>0</v>
+        <v>1543.57142857143</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14140,21 +15541,24 @@
         <f aca="false">$A270+1</f>
         <v>44173</v>
       </c>
+      <c r="B271" s="0" t="n">
+        <v>154740</v>
+      </c>
       <c r="D271" s="1" t="n">
         <f aca="false">B271+C271</f>
-        <v>0</v>
+        <v>154740</v>
       </c>
       <c r="E271" s="1" t="n">
         <f aca="false">D271-D270</f>
-        <v>0</v>
+        <v>1564</v>
       </c>
       <c r="F271" s="1" t="n">
         <f aca="false">(E269+E270+E271)/3</f>
-        <v>0</v>
+        <v>1610.66666666667</v>
       </c>
       <c r="G271" s="1" t="n">
         <f aca="false">(E265+E266+E267+E268+E269+E270+E271)/7</f>
-        <v>0</v>
+        <v>1598.85714285714</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14162,21 +15566,24 @@
         <f aca="false">$A271+1</f>
         <v>44174</v>
       </c>
+      <c r="B272" s="0" t="n">
+        <v>156468</v>
+      </c>
       <c r="D272" s="1" t="n">
         <f aca="false">B272+C272</f>
-        <v>0</v>
+        <v>156468</v>
       </c>
       <c r="E272" s="1" t="n">
         <f aca="false">D272-D271</f>
-        <v>0</v>
+        <v>1728</v>
       </c>
       <c r="F272" s="1" t="n">
         <f aca="false">(E270+E271+E272)/3</f>
-        <v>0</v>
+        <v>1623</v>
       </c>
       <c r="G272" s="1" t="n">
         <f aca="false">(E266+E267+E268+E269+E270+E271+E272)/7</f>
-        <v>0</v>
+        <v>1629.42857142857</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14184,21 +15591,24 @@
         <f aca="false">$A272+1</f>
         <v>44175</v>
       </c>
+      <c r="B273" s="0" t="n">
+        <v>158310</v>
+      </c>
       <c r="D273" s="1" t="n">
         <f aca="false">B273+C273</f>
-        <v>0</v>
+        <v>158310</v>
       </c>
       <c r="E273" s="1" t="n">
         <f aca="false">D273-D272</f>
-        <v>0</v>
+        <v>1842</v>
       </c>
       <c r="F273" s="1" t="n">
         <f aca="false">(E271+E272+E273)/3</f>
-        <v>0</v>
+        <v>1711.33333333333</v>
       </c>
       <c r="G273" s="1" t="n">
         <f aca="false">(E267+E268+E269+E270+E271+E272+E273)/7</f>
-        <v>0</v>
+        <v>1682.57142857143</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14206,21 +15616,24 @@
         <f aca="false">$A273+1</f>
         <v>44176</v>
       </c>
+      <c r="B274" s="0" t="n">
+        <v>160023</v>
+      </c>
       <c r="D274" s="1" t="n">
         <f aca="false">B274+C274</f>
-        <v>0</v>
+        <v>160023</v>
       </c>
       <c r="E274" s="1" t="n">
         <f aca="false">D274-D273</f>
-        <v>0</v>
+        <v>1713</v>
       </c>
       <c r="F274" s="1" t="n">
         <f aca="false">(E272+E273+E274)/3</f>
-        <v>0</v>
+        <v>1761</v>
       </c>
       <c r="G274" s="1" t="n">
         <f aca="false">(E268+E269+E270+E271+E272+E273+E274)/7</f>
-        <v>0</v>
+        <v>1735.14285714286</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14228,21 +15641,24 @@
         <f aca="false">$A274+1</f>
         <v>44177</v>
       </c>
+      <c r="B275" s="0" t="n">
+        <v>161921</v>
+      </c>
       <c r="D275" s="1" t="n">
         <f aca="false">B275+C275</f>
-        <v>0</v>
+        <v>161921</v>
       </c>
       <c r="E275" s="1" t="n">
         <f aca="false">D275-D274</f>
-        <v>0</v>
+        <v>1898</v>
       </c>
       <c r="F275" s="1" t="n">
         <f aca="false">(E273+E274+E275)/3</f>
-        <v>0</v>
+        <v>1817.66666666667</v>
       </c>
       <c r="G275" s="1" t="n">
         <f aca="false">(E269+E270+E271+E272+E273+E274+E275)/7</f>
-        <v>0</v>
+        <v>1716.14285714286</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14250,21 +15666,24 @@
         <f aca="false">$A275+1</f>
         <v>44178</v>
       </c>
+      <c r="B276" s="0" t="n">
+        <v>163915</v>
+      </c>
       <c r="D276" s="1" t="n">
         <f aca="false">B276+C276</f>
-        <v>0</v>
+        <v>163915</v>
       </c>
       <c r="E276" s="1" t="n">
         <f aca="false">D276-D275</f>
-        <v>0</v>
+        <v>1994</v>
       </c>
       <c r="F276" s="1" t="n">
         <f aca="false">(E274+E275+E276)/3</f>
-        <v>0</v>
+        <v>1868.33333333333</v>
       </c>
       <c r="G276" s="1" t="n">
         <f aca="false">(E270+E271+E272+E273+E274+E275+E276)/7</f>
-        <v>0</v>
+        <v>1759.42857142857</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14272,21 +15691,24 @@
         <f aca="false">$A276+1</f>
         <v>44179</v>
       </c>
+      <c r="B277" s="0" t="n">
+        <v>165535</v>
+      </c>
       <c r="D277" s="1" t="n">
         <f aca="false">B277+C277</f>
-        <v>0</v>
+        <v>165535</v>
       </c>
       <c r="E277" s="1" t="n">
         <f aca="false">D277-D276</f>
-        <v>0</v>
+        <v>1620</v>
       </c>
       <c r="F277" s="1" t="n">
         <f aca="false">(E275+E276+E277)/3</f>
-        <v>0</v>
+        <v>1837.33333333333</v>
       </c>
       <c r="G277" s="1" t="n">
         <f aca="false">(E271+E272+E273+E274+E275+E276+E277)/7</f>
-        <v>0</v>
+        <v>1765.57142857143</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14294,21 +15716,24 @@
         <f aca="false">$A277+1</f>
         <v>44180</v>
       </c>
+      <c r="B278" s="0" t="n">
+        <v>167276</v>
+      </c>
       <c r="D278" s="1" t="n">
         <f aca="false">B278+C278</f>
-        <v>0</v>
+        <v>167276</v>
       </c>
       <c r="E278" s="1" t="n">
         <f aca="false">D278-D277</f>
-        <v>0</v>
+        <v>1741</v>
       </c>
       <c r="F278" s="1" t="n">
         <f aca="false">(E276+E277+E278)/3</f>
-        <v>0</v>
+        <v>1785</v>
       </c>
       <c r="G278" s="1" t="n">
         <f aca="false">(E272+E273+E274+E275+E276+E277+E278)/7</f>
-        <v>0</v>
+        <v>1790.85714285714</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14316,21 +15741,24 @@
         <f aca="false">$A278+1</f>
         <v>44181</v>
       </c>
+      <c r="B279" s="0" t="n">
+        <v>169173</v>
+      </c>
       <c r="D279" s="1" t="n">
         <f aca="false">B279+C279</f>
-        <v>0</v>
+        <v>169173</v>
       </c>
       <c r="E279" s="1" t="n">
         <f aca="false">D279-D278</f>
-        <v>0</v>
+        <v>1897</v>
       </c>
       <c r="F279" s="1" t="n">
         <f aca="false">(E277+E278+E279)/3</f>
-        <v>0</v>
+        <v>1752.66666666667</v>
       </c>
       <c r="G279" s="1" t="n">
         <f aca="false">(E273+E274+E275+E276+E277+E278+E279)/7</f>
-        <v>0</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14338,21 +15766,24 @@
         <f aca="false">$A279+1</f>
         <v>44182</v>
       </c>
+      <c r="B280" s="0" t="n">
+        <v>171028</v>
+      </c>
       <c r="D280" s="1" t="n">
         <f aca="false">B280+C280</f>
-        <v>0</v>
+        <v>171028</v>
       </c>
       <c r="E280" s="1" t="n">
         <f aca="false">D280-D279</f>
-        <v>0</v>
+        <v>1855</v>
       </c>
       <c r="F280" s="1" t="n">
         <f aca="false">(E278+E279+E280)/3</f>
-        <v>0</v>
+        <v>1831</v>
       </c>
       <c r="G280" s="1" t="n">
         <f aca="false">(E274+E275+E276+E277+E278+E279+E280)/7</f>
-        <v>0</v>
+        <v>1816.85714285714</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14360,21 +15791,24 @@
         <f aca="false">$A280+1</f>
         <v>44183</v>
       </c>
+      <c r="B281" s="0" t="n">
+        <v>172801</v>
+      </c>
       <c r="D281" s="1" t="n">
         <f aca="false">B281+C281</f>
-        <v>0</v>
+        <v>172801</v>
       </c>
       <c r="E281" s="1" t="n">
         <f aca="false">D281-D280</f>
-        <v>0</v>
+        <v>1773</v>
       </c>
       <c r="F281" s="1" t="n">
         <f aca="false">(E279+E280+E281)/3</f>
-        <v>0</v>
+        <v>1841.66666666667</v>
       </c>
       <c r="G281" s="1" t="n">
         <f aca="false">(E275+E276+E277+E278+E279+E280+E281)/7</f>
-        <v>0</v>
+        <v>1825.42857142857</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14382,21 +15816,24 @@
         <f aca="false">$A281+1</f>
         <v>44184</v>
       </c>
+      <c r="B282" s="0" t="n">
+        <v>174839</v>
+      </c>
       <c r="D282" s="1" t="n">
         <f aca="false">B282+C282</f>
-        <v>0</v>
+        <v>174839</v>
       </c>
       <c r="E282" s="1" t="n">
         <f aca="false">D282-D281</f>
-        <v>0</v>
+        <v>2038</v>
       </c>
       <c r="F282" s="1" t="n">
         <f aca="false">(E280+E281+E282)/3</f>
-        <v>0</v>
+        <v>1888.66666666667</v>
       </c>
       <c r="G282" s="1" t="n">
         <f aca="false">(E276+E277+E278+E279+E280+E281+E282)/7</f>
-        <v>0</v>
+        <v>1845.42857142857</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14404,21 +15841,24 @@
         <f aca="false">$A282+1</f>
         <v>44185</v>
       </c>
+      <c r="B283" s="0" t="n">
+        <v>176985</v>
+      </c>
       <c r="D283" s="1" t="n">
         <f aca="false">B283+C283</f>
-        <v>0</v>
+        <v>176985</v>
       </c>
       <c r="E283" s="1" t="n">
         <f aca="false">D283-D282</f>
-        <v>0</v>
+        <v>2146</v>
       </c>
       <c r="F283" s="1" t="n">
         <f aca="false">(E281+E282+E283)/3</f>
-        <v>0</v>
+        <v>1985.66666666667</v>
       </c>
       <c r="G283" s="1" t="n">
         <f aca="false">(E277+E278+E279+E280+E281+E282+E283)/7</f>
-        <v>0</v>
+        <v>1867.14285714286</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14426,21 +15866,24 @@
         <f aca="false">$A283+1</f>
         <v>44186</v>
       </c>
+      <c r="B284" s="0" t="n">
+        <v>179093</v>
+      </c>
       <c r="D284" s="1" t="n">
         <f aca="false">B284+C284</f>
-        <v>0</v>
+        <v>179093</v>
       </c>
       <c r="E284" s="1" t="n">
         <f aca="false">D284-D283</f>
-        <v>0</v>
+        <v>2108</v>
       </c>
       <c r="F284" s="1" t="n">
         <f aca="false">(E282+E283+E284)/3</f>
-        <v>0</v>
+        <v>2097.33333333333</v>
       </c>
       <c r="G284" s="1" t="n">
         <f aca="false">(E278+E279+E280+E281+E282+E283+E284)/7</f>
-        <v>0</v>
+        <v>1936.85714285714</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14448,21 +15891,24 @@
         <f aca="false">$A284+1</f>
         <v>44187</v>
       </c>
+      <c r="B285" s="0" t="n">
+        <v>181276</v>
+      </c>
       <c r="D285" s="1" t="n">
         <f aca="false">B285+C285</f>
-        <v>0</v>
+        <v>181276</v>
       </c>
       <c r="E285" s="1" t="n">
         <f aca="false">D285-D284</f>
-        <v>0</v>
+        <v>2183</v>
       </c>
       <c r="F285" s="1" t="n">
         <f aca="false">(E283+E284+E285)/3</f>
-        <v>0</v>
+        <v>2145.66666666667</v>
       </c>
       <c r="G285" s="1" t="n">
         <f aca="false">(E279+E280+E281+E282+E283+E284+E285)/7</f>
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14470,21 +15916,24 @@
         <f aca="false">$A285+1</f>
         <v>44188</v>
       </c>
+      <c r="B286" s="0" t="n">
+        <v>183523</v>
+      </c>
       <c r="D286" s="1" t="n">
         <f aca="false">B286+C286</f>
-        <v>0</v>
+        <v>183523</v>
       </c>
       <c r="E286" s="1" t="n">
         <f aca="false">D286-D285</f>
-        <v>0</v>
+        <v>2247</v>
       </c>
       <c r="F286" s="1" t="n">
         <f aca="false">(E284+E285+E286)/3</f>
-        <v>0</v>
+        <v>2179.33333333333</v>
       </c>
       <c r="G286" s="1" t="n">
         <f aca="false">(E280+E281+E282+E283+E284+E285+E286)/7</f>
-        <v>0</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14492,65 +15941,82 @@
         <f aca="false">$A286+1</f>
         <v>44189</v>
       </c>
+      <c r="B287" s="0" t="n">
+        <v>185872</v>
+      </c>
       <c r="D287" s="1" t="n">
         <f aca="false">B287+C287</f>
-        <v>0</v>
+        <v>185872</v>
       </c>
       <c r="E287" s="1" t="n">
         <f aca="false">D287-D286</f>
-        <v>0</v>
+        <v>2349</v>
       </c>
       <c r="F287" s="1" t="n">
         <f aca="false">(E285+E286+E287)/3</f>
-        <v>0</v>
+        <v>2259.66666666667</v>
       </c>
       <c r="G287" s="1" t="n">
         <f aca="false">(E281+E282+E283+E284+E285+E286+E287)/7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2120.57142857143</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="2" t="n">
         <f aca="false">$A287+1</f>
         <v>44190</v>
       </c>
+      <c r="B288" s="0" t="n">
+        <v>185872</v>
+      </c>
+      <c r="C288" s="0" t="n">
+        <f aca="false">((B290-B287)-2291)/2</f>
+        <v>2246</v>
+      </c>
       <c r="D288" s="1" t="n">
         <f aca="false">B288+C288</f>
-        <v>0</v>
+        <v>188118</v>
       </c>
       <c r="E288" s="1" t="n">
         <f aca="false">D288-D287</f>
-        <v>0</v>
+        <v>2246</v>
       </c>
       <c r="F288" s="1" t="n">
         <f aca="false">(E286+E287+E288)/3</f>
-        <v>0</v>
+        <v>2280.66666666667</v>
       </c>
       <c r="G288" s="1" t="n">
         <f aca="false">(E282+E283+E284+E285+E286+E287+E288)/7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2188.14285714286</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="2" t="n">
         <f aca="false">$A288+1</f>
         <v>44191</v>
       </c>
+      <c r="B289" s="0" t="n">
+        <v>185872</v>
+      </c>
+      <c r="C289" s="0" t="n">
+        <f aca="false">(B290-B287)-2291</f>
+        <v>4492</v>
+      </c>
       <c r="D289" s="1" t="n">
         <f aca="false">B289+C289</f>
-        <v>0</v>
+        <v>190364</v>
       </c>
       <c r="E289" s="1" t="n">
         <f aca="false">D289-D288</f>
-        <v>0</v>
+        <v>2246</v>
       </c>
       <c r="F289" s="1" t="n">
         <f aca="false">(E287+E288+E289)/3</f>
-        <v>0</v>
+        <v>2280.33333333333</v>
       </c>
       <c r="G289" s="1" t="n">
         <f aca="false">(E283+E284+E285+E286+E287+E288+E289)/7</f>
-        <v>0</v>
+        <v>2217.85714285714</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14558,21 +16024,24 @@
         <f aca="false">$A289+1</f>
         <v>44192</v>
       </c>
+      <c r="B290" s="0" t="n">
+        <v>192655</v>
+      </c>
       <c r="D290" s="1" t="n">
         <f aca="false">B290+C290</f>
-        <v>0</v>
+        <v>192655</v>
       </c>
       <c r="E290" s="1" t="n">
         <f aca="false">D290-D289</f>
-        <v>0</v>
+        <v>2291</v>
       </c>
       <c r="F290" s="1" t="n">
         <f aca="false">(E288+E289+E290)/3</f>
-        <v>0</v>
+        <v>2261</v>
       </c>
       <c r="G290" s="1" t="n">
         <f aca="false">(E284+E285+E286+E287+E288+E289+E290)/7</f>
-        <v>0</v>
+        <v>2238.57142857143</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14580,43 +16049,52 @@
         <f aca="false">$A290+1</f>
         <v>44193</v>
       </c>
+      <c r="B291" s="0" t="n">
+        <v>194930</v>
+      </c>
       <c r="D291" s="1" t="n">
         <f aca="false">B291+C291</f>
-        <v>0</v>
+        <v>194930</v>
       </c>
       <c r="E291" s="1" t="n">
         <f aca="false">D291-D290</f>
-        <v>0</v>
+        <v>2275</v>
       </c>
       <c r="F291" s="1" t="n">
         <f aca="false">(E289+E290+E291)/3</f>
-        <v>0</v>
+        <v>2270.66666666667</v>
       </c>
       <c r="G291" s="1" t="n">
         <f aca="false">(E285+E286+E287+E288+E289+E290+E291)/7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2262.42857142857</v>
+      </c>
+      <c r="H291" s="0" t="n">
+        <v>2327</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="2" t="n">
         <f aca="false">$A291+1</f>
         <v>44194</v>
       </c>
+      <c r="B292" s="0" t="n">
+        <v>197311</v>
+      </c>
       <c r="D292" s="1" t="n">
         <f aca="false">B292+C292</f>
-        <v>0</v>
+        <v>197311</v>
       </c>
       <c r="E292" s="1" t="n">
         <f aca="false">D292-D291</f>
-        <v>0</v>
+        <v>2381</v>
       </c>
       <c r="F292" s="1" t="n">
         <f aca="false">(E290+E291+E292)/3</f>
-        <v>0</v>
+        <v>2315.66666666667</v>
       </c>
       <c r="G292" s="1" t="n">
         <f aca="false">(E286+E287+E288+E289+E290+E291+E292)/7</f>
-        <v>0</v>
+        <v>2290.71428571429</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14624,21 +16102,24 @@
         <f aca="false">$A292+1</f>
         <v>44195</v>
       </c>
+      <c r="B293" s="0" t="n">
+        <v>199822</v>
+      </c>
       <c r="D293" s="1" t="n">
         <f aca="false">B293+C293</f>
-        <v>0</v>
+        <v>199822</v>
       </c>
       <c r="E293" s="1" t="n">
         <f aca="false">D293-D292</f>
-        <v>0</v>
+        <v>2511</v>
       </c>
       <c r="F293" s="1" t="n">
         <f aca="false">(E291+E292+E293)/3</f>
-        <v>0</v>
+        <v>2389</v>
       </c>
       <c r="G293" s="1" t="n">
         <f aca="false">(E287+E288+E289+E290+E291+E292+E293)/7</f>
-        <v>0</v>
+        <v>2328.42857142857</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14646,65 +16127,81 @@
         <f aca="false">$A293+1</f>
         <v>44196</v>
       </c>
+      <c r="B294" s="0" t="n">
+        <v>202641</v>
+      </c>
       <c r="D294" s="1" t="n">
         <f aca="false">B294+C294</f>
-        <v>0</v>
+        <v>202641</v>
       </c>
       <c r="E294" s="1" t="n">
         <f aca="false">D294-D293</f>
-        <v>0</v>
+        <v>2819</v>
       </c>
       <c r="F294" s="1" t="n">
         <f aca="false">(E292+E293+E294)/3</f>
-        <v>0</v>
+        <v>2570.33333333333</v>
       </c>
       <c r="G294" s="1" t="n">
         <f aca="false">(E288+E289+E290+E291+E292+E293+E294)/7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2395.57142857143</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="2" t="n">
         <f aca="false">$A294+1</f>
         <v>44197</v>
       </c>
+      <c r="B295" s="0" t="n">
+        <v>202641</v>
+      </c>
+      <c r="C295" s="0" t="n">
+        <v>2808</v>
+      </c>
       <c r="D295" s="1" t="n">
         <f aca="false">B295+C295</f>
-        <v>0</v>
+        <v>205449</v>
       </c>
       <c r="E295" s="1" t="n">
         <f aca="false">D295-D294</f>
-        <v>0</v>
+        <v>2808</v>
       </c>
       <c r="F295" s="1" t="n">
         <f aca="false">(E293+E294+E295)/3</f>
-        <v>0</v>
+        <v>2712.66666666667</v>
       </c>
       <c r="G295" s="1" t="n">
         <f aca="false">(E289+E290+E291+E292+E293+E294+E295)/7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2475.85714285714</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="2" t="n">
         <f aca="false">$A295+1</f>
         <v>44198</v>
       </c>
+      <c r="B296" s="0" t="n">
+        <v>202641</v>
+      </c>
+      <c r="C296" s="0" t="n">
+        <f aca="false">C295+1986</f>
+        <v>4794</v>
+      </c>
       <c r="D296" s="1" t="n">
         <f aca="false">B296+C296</f>
-        <v>0</v>
+        <v>207435</v>
       </c>
       <c r="E296" s="1" t="n">
         <f aca="false">D296-D295</f>
-        <v>0</v>
+        <v>1986</v>
       </c>
       <c r="F296" s="1" t="n">
         <f aca="false">(E294+E295+E296)/3</f>
-        <v>0</v>
+        <v>2537.66666666667</v>
       </c>
       <c r="G296" s="1" t="n">
         <f aca="false">(E290+E291+E292+E293+E294+E295+E296)/7</f>
-        <v>0</v>
+        <v>2438.71428571429</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14712,21 +16209,24 @@
         <f aca="false">$A296+1</f>
         <v>44199</v>
       </c>
+      <c r="B297" s="0" t="n">
+        <v>210304</v>
+      </c>
       <c r="D297" s="1" t="n">
         <f aca="false">B297+C297</f>
-        <v>0</v>
+        <v>210304</v>
       </c>
       <c r="E297" s="1" t="n">
         <f aca="false">D297-D296</f>
-        <v>0</v>
+        <v>2869</v>
       </c>
       <c r="F297" s="1" t="n">
         <f aca="false">(E295+E296+E297)/3</f>
-        <v>0</v>
+        <v>2554.33333333333</v>
       </c>
       <c r="G297" s="1" t="n">
         <f aca="false">(E291+E292+E293+E294+E295+E296+E297)/7</f>
-        <v>0</v>
+        <v>2521.28571428571</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14734,21 +16234,24 @@
         <f aca="false">$A297+1</f>
         <v>44200</v>
       </c>
+      <c r="B298" s="0" t="n">
+        <v>212850</v>
+      </c>
       <c r="D298" s="1" t="n">
         <f aca="false">B298+C298</f>
-        <v>0</v>
+        <v>212850</v>
       </c>
       <c r="E298" s="1" t="n">
         <f aca="false">D298-D297</f>
-        <v>0</v>
+        <v>2546</v>
       </c>
       <c r="F298" s="1" t="n">
         <f aca="false">(E296+E297+E298)/3</f>
-        <v>0</v>
+        <v>2467</v>
       </c>
       <c r="G298" s="1" t="n">
         <f aca="false">(E292+E293+E294+E295+E296+E297+E298)/7</f>
-        <v>0</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14756,21 +16259,24 @@
         <f aca="false">$A298+1</f>
         <v>44201</v>
       </c>
+      <c r="B299" s="0" t="n">
+        <v>215358</v>
+      </c>
       <c r="D299" s="1" t="n">
         <f aca="false">B299+C299</f>
-        <v>0</v>
+        <v>215358</v>
       </c>
       <c r="E299" s="1" t="n">
         <f aca="false">D299-D298</f>
-        <v>0</v>
+        <v>2508</v>
       </c>
       <c r="F299" s="1" t="n">
         <f aca="false">(E297+E298+E299)/3</f>
-        <v>0</v>
+        <v>2641</v>
       </c>
       <c r="G299" s="1" t="n">
         <f aca="false">(E293+E294+E295+E296+E297+E298+E299)/7</f>
-        <v>0</v>
+        <v>2578.14285714286</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14778,20 +16284,725 @@
         <f aca="false">$A299+1</f>
         <v>44202</v>
       </c>
+      <c r="B300" s="0" t="n">
+        <v>217999</v>
+      </c>
       <c r="D300" s="1" t="n">
         <f aca="false">B300+C300</f>
-        <v>0</v>
+        <v>217999</v>
       </c>
       <c r="E300" s="1" t="n">
         <f aca="false">D300-D299</f>
-        <v>0</v>
+        <v>2641</v>
       </c>
       <c r="F300" s="1" t="n">
         <f aca="false">(E298+E299+E300)/3</f>
-        <v>0</v>
+        <v>2565</v>
       </c>
       <c r="G300" s="1" t="n">
         <f aca="false">(E294+E295+E296+E297+E298+E299+E300)/7</f>
+        <v>2596.71428571429</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="2" t="n">
+        <f aca="false">$A300+1</f>
+        <v>44203</v>
+      </c>
+      <c r="B301" s="0" t="n">
+        <v>220518</v>
+      </c>
+      <c r="D301" s="1" t="n">
+        <f aca="false">B301+C301</f>
+        <v>220518</v>
+      </c>
+      <c r="E301" s="1" t="n">
+        <f aca="false">D301-D300</f>
+        <v>2519</v>
+      </c>
+      <c r="F301" s="1" t="n">
+        <f aca="false">(E299+E300+E301)/3</f>
+        <v>2556</v>
+      </c>
+      <c r="G301" s="1" t="n">
+        <f aca="false">(E295+E296+E297+E298+E299+E300+E301)/7</f>
+        <v>2553.85714285714</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="2" t="n">
+        <f aca="false">$A301+1</f>
+        <v>44204</v>
+      </c>
+      <c r="B302" s="0" t="n">
+        <v>223106</v>
+      </c>
+      <c r="D302" s="1" t="n">
+        <f aca="false">B302+C302</f>
+        <v>223106</v>
+      </c>
+      <c r="E302" s="1" t="n">
+        <f aca="false">D302-D301</f>
+        <v>2588</v>
+      </c>
+      <c r="F302" s="1" t="n">
+        <f aca="false">(E300+E301+E302)/3</f>
+        <v>2582.66666666667</v>
+      </c>
+      <c r="G302" s="1" t="n">
+        <f aca="false">(E296+E297+E298+E299+E300+E301+E302)/7</f>
+        <v>2522.42857142857</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="2" t="n">
+        <f aca="false">$A302+1</f>
+        <v>44205</v>
+      </c>
+      <c r="B303" s="0" t="n">
+        <v>226233</v>
+      </c>
+      <c r="D303" s="1" t="n">
+        <f aca="false">B303+C303</f>
+        <v>226233</v>
+      </c>
+      <c r="E303" s="1" t="n">
+        <f aca="false">D303-D302</f>
+        <v>3127</v>
+      </c>
+      <c r="F303" s="1" t="n">
+        <f aca="false">(E301+E302+E303)/3</f>
+        <v>2744.66666666667</v>
+      </c>
+      <c r="G303" s="1" t="n">
+        <f aca="false">(E297+E298+E299+E300+E301+E302+E303)/7</f>
+        <v>2685.42857142857</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="2" t="n">
+        <f aca="false">$A303+1</f>
+        <v>44206</v>
+      </c>
+      <c r="B304" s="0" t="n">
+        <v>228821</v>
+      </c>
+      <c r="D304" s="1" t="n">
+        <f aca="false">B304+C304</f>
+        <v>228821</v>
+      </c>
+      <c r="E304" s="1" t="n">
+        <f aca="false">D304-D303</f>
+        <v>2588</v>
+      </c>
+      <c r="F304" s="1" t="n">
+        <f aca="false">(E302+E303+E304)/3</f>
+        <v>2767.66666666667</v>
+      </c>
+      <c r="G304" s="1" t="n">
+        <f aca="false">(E298+E299+E300+E301+E302+E303+E304)/7</f>
+        <v>2645.28571428571</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="2" t="n">
+        <f aca="false">$A304+1</f>
+        <v>44207</v>
+      </c>
+      <c r="B305" s="0" t="n">
+        <v>230690</v>
+      </c>
+      <c r="D305" s="1" t="n">
+        <f aca="false">B305+C305</f>
+        <v>230690</v>
+      </c>
+      <c r="E305" s="1" t="n">
+        <f aca="false">D305-D304</f>
+        <v>1869</v>
+      </c>
+      <c r="F305" s="1" t="n">
+        <f aca="false">(E303+E304+E305)/3</f>
+        <v>2528</v>
+      </c>
+      <c r="G305" s="1" t="n">
+        <f aca="false">(E299+E300+E301+E302+E303+E304+E305)/7</f>
+        <v>2548.57142857143</v>
+      </c>
+    </row>
+    <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="2" t="n">
+        <f aca="false">$A305+1</f>
+        <v>44208</v>
+      </c>
+      <c r="B306" s="0" t="n">
+        <v>232624</v>
+      </c>
+      <c r="D306" s="1" t="n">
+        <f aca="false">B306+C306</f>
+        <v>232624</v>
+      </c>
+      <c r="E306" s="1" t="n">
+        <f aca="false">D306-D305</f>
+        <v>1934</v>
+      </c>
+      <c r="F306" s="1" t="n">
+        <f aca="false">(E304+E305+E306)/3</f>
+        <v>2130.33333333333</v>
+      </c>
+      <c r="G306" s="1" t="n">
+        <f aca="false">(E300+E301+E302+E303+E304+E305+E306)/7</f>
+        <v>2466.57142857143</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="2" t="n">
+        <f aca="false">$A306+1</f>
+        <v>44209</v>
+      </c>
+      <c r="B307" s="0" t="n">
+        <v>234695</v>
+      </c>
+      <c r="D307" s="1" t="n">
+        <f aca="false">B307+C307</f>
+        <v>234695</v>
+      </c>
+      <c r="E307" s="1" t="n">
+        <f aca="false">D307-D306</f>
+        <v>2071</v>
+      </c>
+      <c r="F307" s="1" t="n">
+        <f aca="false">(E305+E306+E307)/3</f>
+        <v>1958</v>
+      </c>
+      <c r="G307" s="1" t="n">
+        <f aca="false">(E301+E302+E303+E304+E305+E306+E307)/7</f>
+        <v>2385.14285714286</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="2" t="n">
+        <f aca="false">$A307+1</f>
+        <v>44210</v>
+      </c>
+      <c r="B308" s="0" t="n">
+        <v>236827</v>
+      </c>
+      <c r="D308" s="1" t="n">
+        <f aca="false">B308+C308</f>
+        <v>236827</v>
+      </c>
+      <c r="E308" s="1" t="n">
+        <f aca="false">D308-D307</f>
+        <v>2132</v>
+      </c>
+      <c r="F308" s="1" t="n">
+        <f aca="false">(E306+E307+E308)/3</f>
+        <v>2045.66666666667</v>
+      </c>
+      <c r="G308" s="1" t="n">
+        <f aca="false">(E302+E303+E304+E305+E306+E307+E308)/7</f>
+        <v>2329.85714285714</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="2" t="n">
+        <f aca="false">$A308+1</f>
+        <v>44211</v>
+      </c>
+      <c r="B309" s="0" t="n">
+        <v>238745</v>
+      </c>
+      <c r="D309" s="1" t="n">
+        <f aca="false">B309+C309</f>
+        <v>238745</v>
+      </c>
+      <c r="E309" s="1" t="n">
+        <f aca="false">D309-D308</f>
+        <v>1918</v>
+      </c>
+      <c r="F309" s="1" t="n">
+        <f aca="false">(E307+E308+E309)/3</f>
+        <v>2040.33333333333</v>
+      </c>
+      <c r="G309" s="1" t="n">
+        <f aca="false">(E303+E304+E305+E306+E307+E308+E309)/7</f>
+        <v>2234.14285714286</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="2" t="n">
+        <f aca="false">$A309+1</f>
+        <v>44212</v>
+      </c>
+      <c r="B310" s="0" t="n">
+        <v>240970</v>
+      </c>
+      <c r="D310" s="1" t="n">
+        <f aca="false">B310+C310</f>
+        <v>240970</v>
+      </c>
+      <c r="E310" s="1" t="n">
+        <f aca="false">D310-D309</f>
+        <v>2225</v>
+      </c>
+      <c r="F310" s="1" t="n">
+        <f aca="false">(E308+E309+E310)/3</f>
+        <v>2091.66666666667</v>
+      </c>
+      <c r="G310" s="1" t="n">
+        <f aca="false">(E304+E305+E306+E307+E308+E309+E310)/7</f>
+        <v>2105.28571428571</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="2" t="n">
+        <f aca="false">$A310+1</f>
+        <v>44213</v>
+      </c>
+      <c r="B311" s="0" t="n">
+        <v>242714</v>
+      </c>
+      <c r="D311" s="1" t="n">
+        <f aca="false">B311+C311</f>
+        <v>242714</v>
+      </c>
+      <c r="E311" s="1" t="n">
+        <f aca="false">D311-D310</f>
+        <v>1744</v>
+      </c>
+      <c r="F311" s="1" t="n">
+        <f aca="false">(E309+E310+E311)/3</f>
+        <v>1962.33333333333</v>
+      </c>
+      <c r="G311" s="1" t="n">
+        <f aca="false">(E305+E306+E307+E308+E309+E310+E311)/7</f>
+        <v>1984.71428571429</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A312" s="2" t="n">
+        <f aca="false">$A311+1</f>
+        <v>44214</v>
+      </c>
+      <c r="B312" s="0" t="n">
+        <v>244348</v>
+      </c>
+      <c r="D312" s="1" t="n">
+        <f aca="false">B312+C312</f>
+        <v>244348</v>
+      </c>
+      <c r="E312" s="1" t="n">
+        <f aca="false">D312-D311</f>
+        <v>1634</v>
+      </c>
+      <c r="F312" s="1" t="n">
+        <f aca="false">(E310+E311+E312)/3</f>
+        <v>1867.66666666667</v>
+      </c>
+      <c r="G312" s="1" t="n">
+        <f aca="false">(E306+E307+E308+E309+E310+E311+E312)/7</f>
+        <v>1951.14285714286</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="2" t="n">
+        <f aca="false">$A312+1</f>
+        <v>44215</v>
+      </c>
+      <c r="B313" s="0" t="n">
+        <v>245734</v>
+      </c>
+      <c r="D313" s="1" t="n">
+        <f aca="false">B313+C313</f>
+        <v>245734</v>
+      </c>
+      <c r="E313" s="1" t="n">
+        <f aca="false">D313-D312</f>
+        <v>1386</v>
+      </c>
+      <c r="F313" s="1" t="n">
+        <f aca="false">(E311+E312+E313)/3</f>
+        <v>1588</v>
+      </c>
+      <c r="G313" s="1" t="n">
+        <f aca="false">(E307+E308+E309+E310+E311+E312+E313)/7</f>
+        <v>1872.85714285714</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="2" t="n">
+        <f aca="false">$A313+1</f>
+        <v>44216</v>
+      </c>
+      <c r="B314" s="0" t="n">
+        <v>247236</v>
+      </c>
+      <c r="D314" s="1" t="n">
+        <f aca="false">B314+C314</f>
+        <v>247236</v>
+      </c>
+      <c r="E314" s="1" t="n">
+        <f aca="false">D314-D313</f>
+        <v>1502</v>
+      </c>
+      <c r="F314" s="1" t="n">
+        <f aca="false">(E312+E313+E314)/3</f>
+        <v>1507.33333333333</v>
+      </c>
+      <c r="G314" s="1" t="n">
+        <f aca="false">(E308+E309+E310+E311+E312+E313+E314)/7</f>
+        <v>1791.57142857143</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="2" t="n">
+        <f aca="false">$A314+1</f>
+        <v>44217</v>
+      </c>
+      <c r="D315" s="1" t="n">
+        <f aca="false">B315+C315</f>
+        <v>0</v>
+      </c>
+      <c r="E315" s="1" t="n">
+        <f aca="false">D315-D314</f>
+        <v>-247236</v>
+      </c>
+      <c r="F315" s="1" t="n">
+        <f aca="false">(E313+E314+E315)/3</f>
+        <v>-81449.3333333333</v>
+      </c>
+      <c r="G315" s="1" t="n">
+        <f aca="false">(E309+E310+E311+E312+E313+E314+E315)/7</f>
+        <v>-33832.4285714286</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="2" t="n">
+        <f aca="false">$A315+1</f>
+        <v>44218</v>
+      </c>
+      <c r="D316" s="1" t="n">
+        <f aca="false">B316+C316</f>
+        <v>0</v>
+      </c>
+      <c r="E316" s="1" t="n">
+        <f aca="false">D316-D315</f>
+        <v>0</v>
+      </c>
+      <c r="F316" s="1" t="n">
+        <f aca="false">(E314+E315+E316)/3</f>
+        <v>-81911.3333333333</v>
+      </c>
+      <c r="G316" s="1" t="n">
+        <f aca="false">(E310+E311+E312+E313+E314+E315+E316)/7</f>
+        <v>-34106.4285714286</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="2" t="n">
+        <f aca="false">$A316+1</f>
+        <v>44219</v>
+      </c>
+      <c r="D317" s="1" t="n">
+        <f aca="false">B317+C317</f>
+        <v>0</v>
+      </c>
+      <c r="E317" s="1" t="n">
+        <f aca="false">D317-D316</f>
+        <v>0</v>
+      </c>
+      <c r="F317" s="1" t="n">
+        <f aca="false">(E315+E316+E317)/3</f>
+        <v>-82412</v>
+      </c>
+      <c r="G317" s="1" t="n">
+        <f aca="false">(E311+E312+E313+E314+E315+E316+E317)/7</f>
+        <v>-34424.2857142857</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="2" t="n">
+        <f aca="false">$A317+1</f>
+        <v>44220</v>
+      </c>
+      <c r="D318" s="1" t="n">
+        <f aca="false">B318+C318</f>
+        <v>0</v>
+      </c>
+      <c r="E318" s="1" t="n">
+        <f aca="false">D318-D317</f>
+        <v>0</v>
+      </c>
+      <c r="F318" s="1" t="n">
+        <f aca="false">(E316+E317+E318)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G318" s="1" t="n">
+        <f aca="false">(E312+E313+E314+E315+E316+E317+E318)/7</f>
+        <v>-34673.4285714286</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A319" s="2" t="n">
+        <f aca="false">$A318+1</f>
+        <v>44221</v>
+      </c>
+      <c r="D319" s="1" t="n">
+        <f aca="false">B319+C319</f>
+        <v>0</v>
+      </c>
+      <c r="E319" s="1" t="n">
+        <f aca="false">D319-D318</f>
+        <v>0</v>
+      </c>
+      <c r="F319" s="1" t="n">
+        <f aca="false">(E317+E318+E319)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G319" s="1" t="n">
+        <f aca="false">(E313+E314+E315+E316+E317+E318+E319)/7</f>
+        <v>-34906.8571428571</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="2" t="n">
+        <f aca="false">$A319+1</f>
+        <v>44222</v>
+      </c>
+      <c r="D320" s="1" t="n">
+        <f aca="false">B320+C320</f>
+        <v>0</v>
+      </c>
+      <c r="E320" s="1" t="n">
+        <f aca="false">D320-D319</f>
+        <v>0</v>
+      </c>
+      <c r="F320" s="1" t="n">
+        <f aca="false">(E318+E319+E320)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G320" s="1" t="n">
+        <f aca="false">(E314+E315+E316+E317+E318+E319+E320)/7</f>
+        <v>-35104.8571428571</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="2" t="n">
+        <f aca="false">$A320+1</f>
+        <v>44223</v>
+      </c>
+      <c r="D321" s="1" t="n">
+        <f aca="false">B321+C321</f>
+        <v>0</v>
+      </c>
+      <c r="E321" s="1" t="n">
+        <f aca="false">D321-D320</f>
+        <v>0</v>
+      </c>
+      <c r="F321" s="1" t="n">
+        <f aca="false">(E319+E320+E321)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G321" s="1" t="n">
+        <f aca="false">(E315+E316+E317+E318+E319+E320+E321)/7</f>
+        <v>-35319.4285714286</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="2" t="n">
+        <f aca="false">$A321+1</f>
+        <v>44224</v>
+      </c>
+      <c r="D322" s="1" t="n">
+        <f aca="false">B322+C322</f>
+        <v>0</v>
+      </c>
+      <c r="E322" s="1" t="n">
+        <f aca="false">D322-D321</f>
+        <v>0</v>
+      </c>
+      <c r="F322" s="1" t="n">
+        <f aca="false">(E320+E321+E322)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G322" s="1" t="n">
+        <f aca="false">(E316+E317+E318+E319+E320+E321+E322)/7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="2" t="n">
+        <f aca="false">$A322+1</f>
+        <v>44225</v>
+      </c>
+      <c r="D323" s="1" t="n">
+        <f aca="false">B323+C323</f>
+        <v>0</v>
+      </c>
+      <c r="E323" s="1" t="n">
+        <f aca="false">D323-D322</f>
+        <v>0</v>
+      </c>
+      <c r="F323" s="1" t="n">
+        <f aca="false">(E321+E322+E323)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G323" s="1" t="n">
+        <f aca="false">(E317+E318+E319+E320+E321+E322+E323)/7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="2" t="n">
+        <f aca="false">$A323+1</f>
+        <v>44226</v>
+      </c>
+      <c r="D324" s="1" t="n">
+        <f aca="false">B324+C324</f>
+        <v>0</v>
+      </c>
+      <c r="E324" s="1" t="n">
+        <f aca="false">D324-D323</f>
+        <v>0</v>
+      </c>
+      <c r="F324" s="1" t="n">
+        <f aca="false">(E322+E323+E324)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G324" s="1" t="n">
+        <f aca="false">(E318+E319+E320+E321+E322+E323+E324)/7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="2" t="n">
+        <f aca="false">$A324+1</f>
+        <v>44227</v>
+      </c>
+      <c r="D325" s="1" t="n">
+        <f aca="false">B325+C325</f>
+        <v>0</v>
+      </c>
+      <c r="E325" s="1" t="n">
+        <f aca="false">D325-D324</f>
+        <v>0</v>
+      </c>
+      <c r="F325" s="1" t="n">
+        <f aca="false">(E323+E324+E325)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G325" s="1" t="n">
+        <f aca="false">(E319+E320+E321+E322+E323+E324+E325)/7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="2" t="n">
+        <f aca="false">$A325+1</f>
+        <v>44228</v>
+      </c>
+      <c r="D326" s="1" t="n">
+        <f aca="false">B326+C326</f>
+        <v>0</v>
+      </c>
+      <c r="E326" s="1" t="n">
+        <f aca="false">D326-D325</f>
+        <v>0</v>
+      </c>
+      <c r="F326" s="1" t="n">
+        <f aca="false">(E324+E325+E326)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G326" s="1" t="n">
+        <f aca="false">(E320+E321+E322+E323+E324+E325+E326)/7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="2" t="n">
+        <f aca="false">$A326+1</f>
+        <v>44229</v>
+      </c>
+      <c r="D327" s="1" t="n">
+        <f aca="false">B327+C327</f>
+        <v>0</v>
+      </c>
+      <c r="E327" s="1" t="n">
+        <f aca="false">D327-D326</f>
+        <v>0</v>
+      </c>
+      <c r="F327" s="1" t="n">
+        <f aca="false">(E325+E326+E327)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G327" s="1" t="n">
+        <f aca="false">(E321+E322+E323+E324+E325+E326+E327)/7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="2" t="n">
+        <f aca="false">$A327+1</f>
+        <v>44230</v>
+      </c>
+      <c r="D328" s="1" t="n">
+        <f aca="false">B328+C328</f>
+        <v>0</v>
+      </c>
+      <c r="E328" s="1" t="n">
+        <f aca="false">D328-D327</f>
+        <v>0</v>
+      </c>
+      <c r="F328" s="1" t="n">
+        <f aca="false">(E326+E327+E328)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G328" s="1" t="n">
+        <f aca="false">(E322+E323+E324+E325+E326+E327+E328)/7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="2" t="n">
+        <f aca="false">$A328+1</f>
+        <v>44231</v>
+      </c>
+      <c r="D329" s="1" t="n">
+        <f aca="false">B329+C329</f>
+        <v>0</v>
+      </c>
+      <c r="E329" s="1" t="n">
+        <f aca="false">D329-D328</f>
+        <v>0</v>
+      </c>
+      <c r="F329" s="1" t="n">
+        <f aca="false">(E327+E328+E329)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G329" s="1" t="n">
+        <f aca="false">(E323+E324+E325+E326+E327+E328+E329)/7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="2" t="n">
+        <f aca="false">$A329+1</f>
+        <v>44232</v>
+      </c>
+      <c r="D330" s="1" t="n">
+        <f aca="false">B330+C330</f>
+        <v>0</v>
+      </c>
+      <c r="E330" s="1" t="n">
+        <f aca="false">D330-D329</f>
+        <v>0</v>
+      </c>
+      <c r="F330" s="1" t="n">
+        <f aca="false">(E328+E329+E330)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G330" s="1" t="n">
+        <f aca="false">(E324+E325+E326+E327+E328+E329+E330)/7</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>